<commit_message>
Updating on Oct 5
</commit_message>
<xml_diff>
--- a/problem1_dataset_values_for_expma_1.xlsx
+++ b/problem1_dataset_values_for_expma_1.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" tabRatio="617" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" tabRatio="617" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$F$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$F$85</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$E$1:$F$63</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet6!$F$1:$G$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet4!$E$1:$F$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet6!$F$1:$G$53</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="100">
   <si>
     <t>JYW:</t>
   </si>
@@ -321,6 +322,24 @@
   <si>
     <t>CELLS</t>
   </si>
+  <si>
+    <t>IFL</t>
+  </si>
+  <si>
+    <t>ZEW</t>
+  </si>
+  <si>
+    <t>CBT</t>
+  </si>
+  <si>
+    <t>VML</t>
+  </si>
+  <si>
+    <t>VTN</t>
+  </si>
+  <si>
+    <t>VKE</t>
+  </si>
 </sst>
 </file>
 
@@ -466,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -546,34 +565,7 @@
     <xf numFmtId="10" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,56 +598,46 @@
     <xf numFmtId="10" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -974,7 +956,7 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A80"/>
+      <selection activeCell="A15" sqref="A15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1241,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1359,7 +1341,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1379,7 +1361,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1419,7 +1401,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -1719,7 +1701,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1759,7 +1741,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
@@ -2059,7 +2041,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
@@ -2119,7 +2101,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -2419,7 +2401,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>72</v>
       </c>
@@ -2559,7 +2541,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>12</v>
       </c>
@@ -2683,10 +2665,6 @@
   <autoFilter ref="A1:F85">
     <filterColumn colId="5">
       <filters>
-        <filter val="0.87"/>
-        <filter val="0.88"/>
-        <filter val="0.89"/>
-        <filter val="0.9"/>
         <filter val="0.91"/>
       </filters>
     </filterColumn>
@@ -2704,7 +2682,7 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A85"/>
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3489,7 +3467,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>39</v>
       </c>
@@ -3589,7 +3567,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>44</v>
       </c>
@@ -3649,7 +3627,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>12</v>
       </c>
@@ -3849,7 +3827,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>57</v>
       </c>
@@ -3969,7 +3947,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>5</v>
       </c>
@@ -4149,7 +4127,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>72</v>
       </c>
@@ -4249,7 +4227,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>77</v>
       </c>
@@ -4269,7 +4247,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>78</v>
       </c>
@@ -4413,9 +4391,6 @@
   <autoFilter ref="A1:F85">
     <filterColumn colId="5">
       <filters>
-        <filter val="0.88"/>
-        <filter val="0.89"/>
-        <filter val="0.9"/>
         <filter val="0.91"/>
       </filters>
     </filterColumn>
@@ -4433,7 +4408,7 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A84"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4638,7 +4613,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -4678,7 +4653,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>73</v>
       </c>
@@ -4778,7 +4753,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -4798,7 +4773,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -5238,7 +5213,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>44</v>
       </c>
@@ -5578,7 +5553,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>57</v>
       </c>
@@ -5678,7 +5653,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>62</v>
       </c>
@@ -5798,7 +5773,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>68</v>
       </c>
@@ -6142,10 +6117,6 @@
   <autoFilter ref="A1:F85">
     <filterColumn colId="5">
       <filters>
-        <filter val="0.85"/>
-        <filter val="0.87"/>
-        <filter val="0.88"/>
-        <filter val="0.89"/>
         <filter val="0.9"/>
       </filters>
     </filterColumn>
@@ -6158,6 +6129,258 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="49"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="49"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="49"/>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="C11" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="C13" s="49"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49"/>
+      <c r="C14" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="51"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="49"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="51"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="C1:C19">
+    <sortCondition ref="C1"/>
+  </sortState>
+  <mergeCells count="10">
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A33:A34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F63"/>
@@ -6215,10 +6438,10 @@
       <c r="C3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="48">
         <v>2</v>
       </c>
     </row>
@@ -6232,8 +6455,8 @@
       <c r="C4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -6245,10 +6468,10 @@
       <c r="C5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="45">
         <v>3</v>
       </c>
     </row>
@@ -6262,8 +6485,8 @@
       <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -6275,8 +6498,8 @@
       <c r="C7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -6288,10 +6511,10 @@
       <c r="C8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="45">
         <v>2</v>
       </c>
     </row>
@@ -6305,8 +6528,8 @@
       <c r="C9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -6318,10 +6541,10 @@
       <c r="C10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="45">
         <v>3</v>
       </c>
     </row>
@@ -6335,8 +6558,8 @@
       <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -6348,8 +6571,8 @@
       <c r="C12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -6378,10 +6601,10 @@
       <c r="C14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="45">
         <v>3</v>
       </c>
     </row>
@@ -6395,8 +6618,8 @@
       <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -6408,8 +6631,8 @@
       <c r="C16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -6421,10 +6644,10 @@
       <c r="C17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="45">
         <v>3</v>
       </c>
     </row>
@@ -6438,8 +6661,8 @@
       <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -6451,8 +6674,8 @@
       <c r="C19" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -6464,10 +6687,10 @@
       <c r="C20" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="45">
         <v>2</v>
       </c>
     </row>
@@ -6475,79 +6698,79 @@
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="31">
+      <c r="F32" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
     </row>
     <row r="34" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E34" s="7" t="s">
@@ -6558,44 +6781,44 @@
       </c>
     </row>
     <row r="35" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="31">
+      <c r="F35" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
     </row>
     <row r="37" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
     </row>
     <row r="38" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F38" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
     </row>
     <row r="40" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="F40" s="31">
+      <c r="F40" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
     </row>
     <row r="42" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E42" s="7" t="s">
@@ -6614,104 +6837,104 @@
       </c>
     </row>
     <row r="44" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="31">
+      <c r="F44" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
     </row>
     <row r="46" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F46" s="31">
+      <c r="F46" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
     </row>
     <row r="48" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
     </row>
     <row r="49" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="34">
+      <c r="F49" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
     </row>
     <row r="51" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
     </row>
     <row r="52" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E52" s="31" t="s">
+      <c r="E52" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="F52" s="31">
+      <c r="F52" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="53" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
     </row>
     <row r="54" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="31" t="s">
+      <c r="E54" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F54" s="31">
+      <c r="F54" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
     </row>
     <row r="56" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
     </row>
     <row r="57" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E57" s="31" t="s">
+      <c r="E57" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F57" s="31">
+      <c r="F57" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
     </row>
     <row r="59" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
     </row>
     <row r="60" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E60" s="31" t="s">
+      <c r="E60" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F60" s="31">
+      <c r="F60" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
     </row>
     <row r="62" spans="5:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E62" s="7" t="s">
@@ -6743,11 +6966,33 @@
     <sortCondition ref="E1"/>
   </sortState>
   <mergeCells count="44">
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F54:F56"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="E60:E61"/>
     <mergeCell ref="F46:F48"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="F20:F21"/>
@@ -6760,39 +7005,17 @@
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="F44:F45"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F60:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
@@ -8142,7 +8365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G53"/>
@@ -8153,7 +8376,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="7" width="9.140625" style="37"/>
+    <col min="6" max="7" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8166,10 +8389,10 @@
       <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="30" t="s">
         <v>93</v>
       </c>
     </row>
@@ -8186,7 +8409,7 @@
       <c r="F2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8203,7 +8426,7 @@
       <c r="F3" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8220,7 +8443,7 @@
       <c r="F4" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8237,7 +8460,7 @@
       <c r="F5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8254,7 +8477,7 @@
       <c r="F6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8271,7 +8494,7 @@
       <c r="F7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8285,10 +8508,10 @@
       <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="50">
         <v>2</v>
       </c>
     </row>
@@ -8302,8 +8525,8 @@
       <c r="C9" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="38"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -8315,10 +8538,10 @@
       <c r="C10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="50">
         <v>2</v>
       </c>
     </row>
@@ -8332,8 +8555,8 @@
       <c r="C11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="38"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -8345,10 +8568,10 @@
       <c r="C12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="50">
         <v>3</v>
       </c>
     </row>
@@ -8362,8 +8585,8 @@
       <c r="C13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="38"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -8375,8 +8598,8 @@
       <c r="C14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="38"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -8388,10 +8611,10 @@
       <c r="C15" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="50">
         <v>2</v>
       </c>
     </row>
@@ -8405,8 +8628,8 @@
       <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="38"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -8418,10 +8641,10 @@
       <c r="C17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="50">
         <v>3</v>
       </c>
     </row>
@@ -8429,18 +8652,18 @@
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="38"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="33"/>
-      <c r="G19" s="38"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8448,7 +8671,7 @@
       <c r="F21" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="37">
+      <c r="G21" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8456,7 +8679,7 @@
       <c r="F22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8464,7 +8687,7 @@
       <c r="F23" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="37">
+      <c r="G23" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8472,7 +8695,7 @@
       <c r="F24" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="37">
+      <c r="G24" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8480,7 +8703,7 @@
       <c r="F25" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="37">
+      <c r="G25" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8488,27 +8711,27 @@
       <c r="F26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="37">
+      <c r="G26" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="31" t="s">
+      <c r="F27" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="38">
+      <c r="G27" s="50">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="33"/>
-      <c r="G28" s="38"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="50"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G29" s="37">
+      <c r="G29" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8516,7 +8739,7 @@
       <c r="F30" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G30" s="37">
+      <c r="G30" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8524,7 +8747,7 @@
       <c r="F31" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="37">
+      <c r="G31" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8532,47 +8755,47 @@
       <c r="F32" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="37">
+      <c r="G32" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="50">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="6:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="33"/>
-      <c r="G34" s="38"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="50"/>
     </row>
     <row r="35" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F35" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="37">
+      <c r="G35" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="50">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="6:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="33"/>
-      <c r="G37" s="38"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="50"/>
     </row>
     <row r="38" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F38" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G38" s="37">
+      <c r="G38" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8580,7 +8803,7 @@
       <c r="F39" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G39" s="37">
+      <c r="G39" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8588,27 +8811,27 @@
       <c r="F40" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="37">
+      <c r="G40" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="G41" s="38">
+      <c r="G41" s="50">
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="6:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="33"/>
-      <c r="G42" s="38"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="50"/>
     </row>
     <row r="43" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F43" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G43" s="37">
+      <c r="G43" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8616,63 +8839,63 @@
       <c r="F44" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G44" s="37">
+      <c r="G44" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="G45" s="38">
+      <c r="G45" s="50">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="6:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="F46" s="32"/>
-      <c r="G46" s="38"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="50"/>
     </row>
     <row r="47" spans="6:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F47" s="33"/>
-      <c r="G47" s="38"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="50"/>
     </row>
     <row r="48" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F48" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="37">
+      <c r="G48" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F49" s="31" t="s">
+      <c r="F49" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="50">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="6:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="33"/>
-      <c r="G50" s="38"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="50"/>
     </row>
     <row r="51" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F51" s="29" t="s">
+      <c r="F51" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="G51" s="38">
+      <c r="G51" s="50">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="6:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F52" s="30"/>
-      <c r="G52" s="38"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="50"/>
     </row>
     <row r="53" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F53" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G53" s="37">
+      <c r="G53" s="29">
         <v>1</v>
       </c>
     </row>
@@ -8688,11 +8911,18 @@
     <sortCondition ref="D1"/>
   </sortState>
   <mergeCells count="24">
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G45:G47"/>
-    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="F49:F50"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
@@ -8700,1422 +8930,1415 @@
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="G17:G19"/>
     <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G45:G47"/>
+    <mergeCell ref="G49:G50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:T22"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="50">
+      <c r="B1" s="41">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="C1" s="49">
+      <c r="C1" s="40">
         <v>1.6</v>
       </c>
-      <c r="D1" s="49">
+      <c r="D1" s="40">
         <v>0.44</v>
       </c>
-      <c r="E1" s="49">
+      <c r="E1" s="40">
         <v>0.45</v>
       </c>
-      <c r="F1" s="49">
+      <c r="F1" s="40">
         <v>0.9</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="49" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="50">
+      <c r="I1" s="41">
         <v>3.1899999999999998E-2</v>
       </c>
-      <c r="J1" s="49">
+      <c r="J1" s="40">
         <v>1.43</v>
       </c>
-      <c r="K1" s="49">
+      <c r="K1" s="40">
         <v>0.42</v>
       </c>
-      <c r="L1" s="49">
+      <c r="L1" s="40">
         <v>0.44</v>
       </c>
-      <c r="M1" s="49">
+      <c r="M1" s="40">
         <v>0.9</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="49" t="s">
+      <c r="N1" s="36"/>
+      <c r="O1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="50">
+      <c r="P1" s="41">
         <v>5.7799999999999997E-2</v>
       </c>
-      <c r="Q1" s="49">
+      <c r="Q1" s="40">
         <v>1.59</v>
       </c>
-      <c r="R1" s="49">
+      <c r="R1" s="40">
         <v>0.44</v>
       </c>
-      <c r="S1" s="49">
+      <c r="S1" s="40">
         <v>0.51</v>
       </c>
-      <c r="T1" s="49">
+      <c r="T1" s="40">
         <v>0.9</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="44">
-        <v>0</v>
-      </c>
-      <c r="C2" s="43">
+      <c r="B2" s="35">
+        <v>0</v>
+      </c>
+      <c r="C2" s="34">
         <v>1.43</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="34">
         <v>0.4</v>
       </c>
-      <c r="E2" s="43">
+      <c r="E2" s="34">
         <v>0.05</v>
       </c>
-      <c r="F2" s="43">
+      <c r="F2" s="34">
         <v>0.91</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="43" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="44">
+      <c r="I2" s="35">
         <v>1E-4</v>
       </c>
-      <c r="J2" s="43">
+      <c r="J2" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K2" s="43">
+      <c r="K2" s="34">
         <v>0.33</v>
       </c>
-      <c r="L2" s="43">
+      <c r="L2" s="34">
         <v>0.04</v>
       </c>
-      <c r="M2" s="43">
+      <c r="M2" s="34">
         <v>0.93</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="43" t="s">
+      <c r="N2" s="36"/>
+      <c r="O2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="44">
+      <c r="P2" s="35">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="Q2" s="43">
+      <c r="Q2" s="34">
         <v>4.83</v>
       </c>
-      <c r="R2" s="43">
+      <c r="R2" s="34">
         <v>0.5</v>
       </c>
-      <c r="S2" s="43">
+      <c r="S2" s="34">
         <v>0.05</v>
       </c>
-      <c r="T2" s="43">
+      <c r="T2" s="34">
         <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="35">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="34">
         <v>1.78</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="34">
         <v>0.42</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="34">
         <v>0.06</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="34">
         <v>0.92</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="43" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="35">
         <v>1E-4</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="34">
         <v>1.23</v>
       </c>
-      <c r="K3" s="43">
+      <c r="K3" s="34">
         <v>0.44</v>
       </c>
-      <c r="L3" s="43">
+      <c r="L3" s="34">
         <v>0.06</v>
       </c>
-      <c r="M3" s="43">
+      <c r="M3" s="34">
         <v>0.94</v>
       </c>
-      <c r="N3" s="45"/>
-      <c r="O3" s="43" t="s">
+      <c r="N3" s="36"/>
+      <c r="O3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="44">
+      <c r="P3" s="35">
         <v>1E-3</v>
       </c>
-      <c r="Q3" s="43">
+      <c r="Q3" s="34">
         <v>3.72</v>
       </c>
-      <c r="R3" s="43">
+      <c r="R3" s="34">
         <v>0.44</v>
       </c>
-      <c r="S3" s="43">
+      <c r="S3" s="34">
         <v>0.08</v>
       </c>
-      <c r="T3" s="43">
+      <c r="T3" s="34">
         <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="35">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="34">
         <v>2.58</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="34">
         <v>0.5</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="34">
         <v>0.09</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="34">
         <v>0.91</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="43" t="s">
+      <c r="G4" s="36"/>
+      <c r="H4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="44">
+      <c r="I4" s="35">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="34">
         <v>2.09</v>
       </c>
-      <c r="K4" s="43">
+      <c r="K4" s="34">
         <v>0.49</v>
       </c>
-      <c r="L4" s="43">
+      <c r="L4" s="34">
         <v>0.09</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="34">
         <v>0.92</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="43" t="s">
+      <c r="N4" s="36"/>
+      <c r="O4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="35">
         <v>1E-4</v>
       </c>
-      <c r="Q4" s="43">
+      <c r="Q4" s="34">
         <v>1.0900000000000001</v>
       </c>
-      <c r="R4" s="43">
+      <c r="R4" s="34">
         <v>0.4</v>
       </c>
-      <c r="S4" s="43">
+      <c r="S4" s="34">
         <v>0.11</v>
       </c>
-      <c r="T4" s="43">
+      <c r="T4" s="34">
         <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="35">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="34">
         <v>1.92</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="34">
         <v>0.43</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="34">
         <v>0.16</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="34">
         <v>0.92</v>
       </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="43" t="s">
+      <c r="G5" s="36"/>
+      <c r="H5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="35">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="34">
         <v>1.43</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="34">
         <v>0.47</v>
       </c>
-      <c r="L5" s="43">
+      <c r="L5" s="34">
         <v>0.13</v>
       </c>
-      <c r="M5" s="43">
+      <c r="M5" s="34">
         <v>0.91</v>
       </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="43" t="s">
+      <c r="N5" s="36"/>
+      <c r="O5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="35">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="Q5" s="43">
+      <c r="Q5" s="34">
         <v>1.25</v>
       </c>
-      <c r="R5" s="43">
+      <c r="R5" s="34">
         <v>0.42</v>
       </c>
-      <c r="S5" s="43">
+      <c r="S5" s="34">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T5" s="43">
+      <c r="T5" s="34">
         <v>0.91</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="35">
         <v>-1E-4</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="34">
         <v>0.83</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="34">
         <v>0.46</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="34">
         <v>0.08</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="34">
         <v>0.87</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="43" t="s">
+      <c r="G6" s="36"/>
+      <c r="H6" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="44">
+      <c r="I6" s="35">
         <v>1E-4</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="34">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="34">
         <v>0.42</v>
       </c>
-      <c r="L6" s="43">
+      <c r="L6" s="34">
         <v>0.1</v>
       </c>
-      <c r="M6" s="43">
+      <c r="M6" s="34">
         <v>0.93</v>
       </c>
-      <c r="N6" s="45"/>
-      <c r="O6" s="43" t="s">
+      <c r="N6" s="36"/>
+      <c r="O6" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="35">
         <v>1E-4</v>
       </c>
-      <c r="Q6" s="43">
+      <c r="Q6" s="34">
         <v>9.5</v>
       </c>
-      <c r="R6" s="43">
+      <c r="R6" s="34">
         <v>0.5</v>
       </c>
-      <c r="S6" s="43">
+      <c r="S6" s="34">
         <v>0.05</v>
       </c>
-      <c r="T6" s="43">
+      <c r="T6" s="34">
         <v>0.92</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="35">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="34">
         <v>1.2</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="34">
         <v>0.41</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="34">
         <v>0.13</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="34">
         <v>0.89</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="43" t="s">
+      <c r="G7" s="36"/>
+      <c r="H7" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="35">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="34">
         <v>1.17</v>
       </c>
-      <c r="K7" s="43">
+      <c r="K7" s="34">
         <v>0.42</v>
       </c>
-      <c r="L7" s="43">
+      <c r="L7" s="34">
         <v>0.1</v>
       </c>
-      <c r="M7" s="43">
+      <c r="M7" s="34">
         <v>0.88</v>
       </c>
-      <c r="N7" s="45"/>
-      <c r="O7" s="43" t="s">
+      <c r="N7" s="36"/>
+      <c r="O7" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="35">
         <v>1E-4</v>
       </c>
-      <c r="Q7" s="43">
+      <c r="Q7" s="34">
         <v>1.46</v>
       </c>
-      <c r="R7" s="43">
+      <c r="R7" s="34">
         <v>0.44</v>
       </c>
-      <c r="S7" s="43">
+      <c r="S7" s="34">
         <v>0.06</v>
       </c>
-      <c r="T7" s="43">
+      <c r="T7" s="34">
         <v>0.93</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="35">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="34">
         <v>1.5</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="34">
         <v>0.44</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="34">
         <v>0.2</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="34">
         <v>0.9</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="43" t="s">
+      <c r="G8" s="36"/>
+      <c r="H8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="44">
+      <c r="I8" s="35">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="34">
         <v>1.07</v>
       </c>
-      <c r="K8" s="43">
+      <c r="K8" s="34">
         <v>0.4</v>
       </c>
-      <c r="L8" s="43">
+      <c r="L8" s="34">
         <v>0.25</v>
       </c>
-      <c r="M8" s="43">
+      <c r="M8" s="34">
         <v>0.88</v>
       </c>
-      <c r="N8" s="45"/>
-      <c r="O8" s="43" t="s">
+      <c r="N8" s="36"/>
+      <c r="O8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="35">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="Q8" s="43">
+      <c r="Q8" s="34">
         <v>1.29</v>
       </c>
-      <c r="R8" s="43">
+      <c r="R8" s="34">
         <v>0.41</v>
       </c>
-      <c r="S8" s="43">
+      <c r="S8" s="34">
         <v>0.33</v>
       </c>
-      <c r="T8" s="43">
+      <c r="T8" s="34">
         <v>0.88</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="35">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="34">
         <v>2.16</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="34">
         <v>0.47</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="34">
         <v>0.09</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="34">
         <v>0.9</v>
       </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="43" t="s">
+      <c r="G9" s="36"/>
+      <c r="H9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="44">
-        <v>0</v>
-      </c>
-      <c r="J9" s="43">
+      <c r="I9" s="35">
+        <v>0</v>
+      </c>
+      <c r="J9" s="34">
         <v>1.06</v>
       </c>
-      <c r="K9" s="43">
+      <c r="K9" s="34">
         <v>0.47</v>
       </c>
-      <c r="L9" s="43">
+      <c r="L9" s="34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M9" s="43">
+      <c r="M9" s="34">
         <v>0.93</v>
       </c>
-      <c r="N9" s="45"/>
-      <c r="O9" s="43" t="s">
+      <c r="N9" s="36"/>
+      <c r="O9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="35">
         <v>-6.9999999999999999E-4</v>
       </c>
-      <c r="Q9" s="43">
+      <c r="Q9" s="34">
         <v>0.67</v>
       </c>
-      <c r="R9" s="43">
+      <c r="R9" s="34">
         <v>0.36</v>
       </c>
-      <c r="S9" s="43">
+      <c r="S9" s="34">
         <v>0.12</v>
       </c>
-      <c r="T9" s="43">
+      <c r="T9" s="34">
         <v>0.91</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="35">
         <v>1.4E-3</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="34">
         <v>1.44</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="34">
         <v>0.43</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="34">
         <v>0.15</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="34">
         <v>0.89</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="43" t="s">
+      <c r="G10" s="36"/>
+      <c r="H10" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="35">
         <v>-4.0000000000000002E-4</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="34">
         <v>0.81</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="34">
         <v>0.41</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="34">
         <v>0.13</v>
       </c>
-      <c r="M10" s="43">
+      <c r="M10" s="34">
         <v>0.88</v>
       </c>
-      <c r="N10" s="45"/>
-      <c r="O10" s="43" t="s">
+      <c r="N10" s="36"/>
+      <c r="O10" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="35">
         <v>1.4E-3</v>
       </c>
-      <c r="Q10" s="43">
+      <c r="Q10" s="34">
         <v>2.95</v>
       </c>
-      <c r="R10" s="43">
+      <c r="R10" s="34">
         <v>0.46</v>
       </c>
-      <c r="S10" s="43">
+      <c r="S10" s="34">
         <v>0.12</v>
       </c>
-      <c r="T10" s="43">
+      <c r="T10" s="34">
         <v>0.89</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="35">
         <v>1.32E-2</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="34">
         <v>1.63</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="34">
         <v>0.44</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="34">
         <v>0.23</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="34">
         <v>0.91</v>
       </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="43" t="s">
+      <c r="G11" s="36"/>
+      <c r="H11" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="44">
+      <c r="I11" s="35">
         <v>1.29E-2</v>
       </c>
-      <c r="J11" s="43">
+      <c r="J11" s="34">
         <v>1.99</v>
       </c>
-      <c r="K11" s="43">
+      <c r="K11" s="34">
         <v>0.44</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="34">
         <v>0.23</v>
       </c>
-      <c r="M11" s="43">
+      <c r="M11" s="34">
         <v>0.92</v>
       </c>
-      <c r="N11" s="45"/>
-      <c r="O11" s="43" t="s">
+      <c r="N11" s="36"/>
+      <c r="O11" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="P11" s="44">
+      <c r="P11" s="35">
         <v>1.95E-2</v>
       </c>
-      <c r="Q11" s="43">
+      <c r="Q11" s="34">
         <v>1.77</v>
       </c>
-      <c r="R11" s="43">
+      <c r="R11" s="34">
         <v>0.45</v>
       </c>
-      <c r="S11" s="43">
+      <c r="S11" s="34">
         <v>0.3</v>
       </c>
-      <c r="T11" s="43">
+      <c r="T11" s="34">
         <v>0.92</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="35">
         <v>1E-4</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="34">
         <v>1.03</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="34">
         <v>0.43</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="34">
         <v>0.13</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="34">
         <v>0.91</v>
       </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="43" t="s">
+      <c r="G12" s="36"/>
+      <c r="H12" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="44">
-        <v>0</v>
-      </c>
-      <c r="J12" s="43">
+      <c r="I12" s="35">
+        <v>0</v>
+      </c>
+      <c r="J12" s="34">
         <v>0.99</v>
       </c>
-      <c r="K12" s="43">
+      <c r="K12" s="34">
         <v>0.45</v>
       </c>
-      <c r="L12" s="43">
+      <c r="L12" s="34">
         <v>0.15</v>
       </c>
-      <c r="M12" s="43">
+      <c r="M12" s="34">
         <v>0.91</v>
       </c>
-      <c r="N12" s="45"/>
-      <c r="O12" s="43" t="s">
+      <c r="N12" s="36"/>
+      <c r="O12" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="44">
+      <c r="P12" s="35">
         <v>2.8E-3</v>
       </c>
-      <c r="Q12" s="43">
+      <c r="Q12" s="34">
         <v>2.3199999999999998</v>
       </c>
-      <c r="R12" s="43">
+      <c r="R12" s="34">
         <v>0.48</v>
       </c>
-      <c r="S12" s="43">
+      <c r="S12" s="34">
         <v>0.14000000000000001</v>
       </c>
-      <c r="T12" s="43">
+      <c r="T12" s="34">
         <v>0.92</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="38">
         <v>1E-4</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="37">
         <v>1.23</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="37">
         <v>0.45</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="37">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="37">
         <v>0.92</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="46" t="s">
+      <c r="G13" s="39"/>
+      <c r="H13" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="38">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="J13" s="46">
+      <c r="J13" s="37">
         <v>1.61</v>
       </c>
-      <c r="K13" s="46">
+      <c r="K13" s="37">
         <v>0.38</v>
       </c>
-      <c r="L13" s="46">
+      <c r="L13" s="37">
         <v>0.08</v>
       </c>
-      <c r="M13" s="46">
+      <c r="M13" s="37">
         <v>0.91</v>
       </c>
-      <c r="N13" s="48"/>
-      <c r="O13" s="46" t="s">
+      <c r="N13" s="39"/>
+      <c r="O13" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="38">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="Q13" s="46">
+      <c r="Q13" s="37">
         <v>1.67</v>
       </c>
-      <c r="R13" s="46">
+      <c r="R13" s="37">
         <v>0.42</v>
       </c>
-      <c r="S13" s="46">
+      <c r="S13" s="37">
         <v>0.09</v>
       </c>
-      <c r="T13" s="46">
+      <c r="T13" s="37">
         <v>0.92</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="35">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="34">
         <v>1.81</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="34">
         <v>0.44</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="34">
         <v>0.08</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="34">
         <v>0.91</v>
       </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="43" t="s">
+      <c r="G14" s="36"/>
+      <c r="H14" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="44">
+      <c r="I14" s="35">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="J14" s="43">
+      <c r="J14" s="34">
         <v>3.06</v>
       </c>
-      <c r="K14" s="43">
+      <c r="K14" s="34">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="34">
         <v>0.08</v>
       </c>
-      <c r="M14" s="43">
+      <c r="M14" s="34">
         <v>0.91</v>
       </c>
-      <c r="N14" s="45"/>
-      <c r="O14" s="43" t="s">
+      <c r="N14" s="36"/>
+      <c r="O14" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="35">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="Q14" s="43">
+      <c r="Q14" s="34">
         <v>2.6</v>
       </c>
-      <c r="R14" s="43">
+      <c r="R14" s="34">
         <v>0.45</v>
       </c>
-      <c r="S14" s="43">
+      <c r="S14" s="34">
         <v>0.09</v>
       </c>
-      <c r="T14" s="43">
+      <c r="T14" s="34">
         <v>0.91</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="44">
-        <v>0</v>
-      </c>
-      <c r="C15" s="43">
+      <c r="B15" s="35">
+        <v>0</v>
+      </c>
+      <c r="C15" s="34">
         <v>0.8</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="34">
         <v>0.47</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="34">
         <v>0.89</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="43" t="s">
+      <c r="G15" s="36"/>
+      <c r="H15" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="35">
         <v>1E-4</v>
       </c>
-      <c r="J15" s="43">
+      <c r="J15" s="34">
         <v>1.35</v>
       </c>
-      <c r="K15" s="43">
+      <c r="K15" s="34">
         <v>0.44</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M15" s="43">
+      <c r="M15" s="34">
         <v>0.89</v>
       </c>
-      <c r="N15" s="45"/>
-      <c r="O15" s="43" t="s">
+      <c r="N15" s="36"/>
+      <c r="O15" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="P15" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="43">
+      <c r="P15" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="34">
         <v>1.25</v>
       </c>
-      <c r="R15" s="43">
+      <c r="R15" s="34">
         <v>0.36</v>
       </c>
-      <c r="S15" s="43">
+      <c r="S15" s="34">
         <v>0.06</v>
       </c>
-      <c r="T15" s="43">
+      <c r="T15" s="34">
         <v>0.91</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B16" s="35">
         <v>1E-4</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="34">
         <v>1.07</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="34">
         <v>0.39</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="34">
         <v>0.11</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="34">
         <v>0.92</v>
       </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="43" t="s">
+      <c r="G16" s="36"/>
+      <c r="H16" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="I16" s="44">
+      <c r="I16" s="35">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="J16" s="43">
+      <c r="J16" s="34">
         <v>1.59</v>
       </c>
-      <c r="K16" s="43">
+      <c r="K16" s="34">
         <v>0.47</v>
       </c>
-      <c r="L16" s="43">
+      <c r="L16" s="34">
         <v>0.1</v>
       </c>
-      <c r="M16" s="43">
+      <c r="M16" s="34">
         <v>0.93</v>
       </c>
-      <c r="N16" s="45"/>
-      <c r="O16" s="43" t="s">
+      <c r="N16" s="36"/>
+      <c r="O16" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="P16" s="44">
+      <c r="P16" s="35">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Q16" s="43">
+      <c r="Q16" s="34">
         <v>2.42</v>
       </c>
-      <c r="R16" s="43">
+      <c r="R16" s="34">
         <v>0.45</v>
       </c>
-      <c r="S16" s="43">
+      <c r="S16" s="34">
         <v>0.13</v>
       </c>
-      <c r="T16" s="43">
+      <c r="T16" s="34">
         <v>0.87</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="35">
         <v>1E-4</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="34">
         <v>1.2</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="34">
         <v>0.41</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="34">
         <v>0.09</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="34">
         <v>0.91</v>
       </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="43" t="s">
+      <c r="G17" s="36"/>
+      <c r="H17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="I17" s="44">
-        <v>0</v>
-      </c>
-      <c r="J17" s="43">
+      <c r="I17" s="35">
+        <v>0</v>
+      </c>
+      <c r="J17" s="34">
         <v>1.01</v>
       </c>
-      <c r="K17" s="43">
+      <c r="K17" s="34">
         <v>0.43</v>
       </c>
-      <c r="L17" s="43">
+      <c r="L17" s="34">
         <v>0.09</v>
       </c>
-      <c r="M17" s="43">
+      <c r="M17" s="34">
         <v>0.91</v>
       </c>
-      <c r="N17" s="45"/>
-      <c r="O17" s="43" t="s">
+      <c r="N17" s="36"/>
+      <c r="O17" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="P17" s="44">
+      <c r="P17" s="35">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="Q17" s="43">
+      <c r="Q17" s="34">
         <v>2.35</v>
       </c>
-      <c r="R17" s="43">
+      <c r="R17" s="34">
         <v>0.48</v>
       </c>
-      <c r="S17" s="43">
+      <c r="S17" s="34">
         <v>0.08</v>
       </c>
-      <c r="T17" s="43">
+      <c r="T17" s="34">
         <v>0.91</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="44">
+      <c r="B18" s="35">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="34">
         <v>1.86</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="34">
         <v>0.47</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="34">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="34">
         <v>0.92</v>
       </c>
-      <c r="G18" s="45"/>
-      <c r="H18" s="43" t="s">
+      <c r="G18" s="36"/>
+      <c r="H18" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="44">
+      <c r="I18" s="35">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="J18" s="43">
+      <c r="J18" s="34">
         <v>1.82</v>
       </c>
-      <c r="K18" s="43">
+      <c r="K18" s="34">
         <v>0.43</v>
       </c>
-      <c r="L18" s="43">
+      <c r="L18" s="34">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M18" s="43">
+      <c r="M18" s="34">
         <v>0.9</v>
       </c>
-      <c r="N18" s="45"/>
-      <c r="O18" s="43" t="s">
+      <c r="N18" s="36"/>
+      <c r="O18" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="35">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Q18" s="43">
+      <c r="Q18" s="34">
         <v>1.59</v>
       </c>
-      <c r="R18" s="43">
+      <c r="R18" s="34">
         <v>0.45</v>
       </c>
-      <c r="S18" s="43">
+      <c r="S18" s="34">
         <v>0.18</v>
       </c>
-      <c r="T18" s="43">
+      <c r="T18" s="34">
         <v>0.9</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="35">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="34">
         <v>1.78</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="34">
         <v>0.46</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="34">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="34">
         <v>0.92</v>
       </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="43" t="s">
+      <c r="G19" s="36"/>
+      <c r="H19" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="35">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="J19" s="43">
+      <c r="J19" s="34">
         <v>1.39</v>
       </c>
-      <c r="K19" s="43">
+      <c r="K19" s="34">
         <v>0.46</v>
       </c>
-      <c r="L19" s="43">
+      <c r="L19" s="34">
         <v>0.12</v>
       </c>
-      <c r="M19" s="43">
+      <c r="M19" s="34">
         <v>0.92</v>
       </c>
-      <c r="N19" s="45"/>
-      <c r="O19" s="43" t="s">
+      <c r="N19" s="36"/>
+      <c r="O19" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="35">
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="Q19" s="43">
+      <c r="Q19" s="34">
         <v>1.82</v>
       </c>
-      <c r="R19" s="43">
+      <c r="R19" s="34">
         <v>0.43</v>
       </c>
-      <c r="S19" s="43">
+      <c r="S19" s="34">
         <v>0.18</v>
       </c>
-      <c r="T19" s="43">
+      <c r="T19" s="34">
         <v>0.9</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="33">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="32">
         <v>1.94</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="32">
         <v>0.45</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="32">
         <v>0.22</v>
       </c>
-      <c r="F20" s="41">
+      <c r="F20" s="32">
         <v>0.93</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41" t="s">
+      <c r="G20" s="31"/>
+      <c r="H20" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="42">
+      <c r="I20" s="33">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="J20" s="41">
+      <c r="J20" s="32">
         <v>1.38</v>
       </c>
-      <c r="K20" s="41">
+      <c r="K20" s="32">
         <v>0.43</v>
       </c>
-      <c r="L20" s="41">
+      <c r="L20" s="32">
         <v>0.24</v>
       </c>
-      <c r="M20" s="41">
+      <c r="M20" s="32">
         <v>0.91</v>
       </c>
-      <c r="N20" s="40"/>
-      <c r="O20" s="41" t="s">
+      <c r="N20" s="31"/>
+      <c r="O20" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P20" s="42">
+      <c r="P20" s="33">
         <v>1.37E-2</v>
       </c>
-      <c r="Q20" s="41">
+      <c r="Q20" s="32">
         <v>1.61</v>
       </c>
-      <c r="R20" s="41">
+      <c r="R20" s="32">
         <v>0.44</v>
       </c>
-      <c r="S20" s="41">
+      <c r="S20" s="32">
         <v>0.26</v>
       </c>
-      <c r="T20" s="41">
+      <c r="T20" s="32">
         <v>0.92</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="33">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="32">
         <v>2.36</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="32">
         <v>0.48</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="32">
         <v>0.15</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="32">
         <v>0.92</v>
       </c>
-      <c r="G21" s="40"/>
-      <c r="H21" s="41" t="s">
+      <c r="G21" s="31"/>
+      <c r="H21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I21" s="33">
         <v>5.4800000000000001E-2</v>
       </c>
-      <c r="J21" s="41">
+      <c r="J21" s="32">
         <v>1.75</v>
       </c>
-      <c r="K21" s="41">
+      <c r="K21" s="32">
         <v>0.44</v>
       </c>
-      <c r="L21" s="41">
+      <c r="L21" s="32">
         <v>0.47</v>
       </c>
-      <c r="M21" s="41">
+      <c r="M21" s="32">
         <v>0.89</v>
       </c>
-      <c r="N21" s="40"/>
-      <c r="O21" s="41" t="s">
+      <c r="N21" s="31"/>
+      <c r="O21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="P21" s="42">
+      <c r="P21" s="33">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="Q21" s="41">
+      <c r="Q21" s="32">
         <v>2.74</v>
       </c>
-      <c r="R21" s="41">
+      <c r="R21" s="32">
         <v>0.47</v>
       </c>
-      <c r="S21" s="41">
+      <c r="S21" s="32">
         <v>0.12</v>
       </c>
-      <c r="T21" s="41">
+      <c r="T21" s="32">
         <v>0.94</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="44">
-        <v>0</v>
-      </c>
-      <c r="C22" s="43">
+      <c r="B22" s="35">
+        <v>0</v>
+      </c>
+      <c r="C22" s="34">
         <v>0.9</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="34">
         <v>0.33</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="34">
         <v>0.05</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="34">
         <v>0.93</v>
       </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="43" t="s">
+      <c r="G22" s="36"/>
+      <c r="H22" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="I22" s="44">
-        <v>0</v>
-      </c>
-      <c r="J22" s="43">
+      <c r="I22" s="35">
+        <v>0</v>
+      </c>
+      <c r="J22" s="34">
         <v>1.5</v>
       </c>
-      <c r="K22" s="43">
+      <c r="K22" s="34">
         <v>0.67</v>
       </c>
-      <c r="L22" s="43">
+      <c r="L22" s="34">
         <v>0.06</v>
       </c>
-      <c r="M22" s="43">
+      <c r="M22" s="34">
         <v>0.92</v>
       </c>
-      <c r="N22" s="45"/>
-      <c r="O22" s="43" t="s">
+      <c r="N22" s="36"/>
+      <c r="O22" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="44">
+      <c r="P22" s="35">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="Q22" s="43">
+      <c r="Q22" s="34">
         <v>4.08</v>
       </c>
-      <c r="R22" s="43">
+      <c r="R22" s="34">
         <v>0.5</v>
       </c>
-      <c r="S22" s="43">
+      <c r="S22" s="34">
         <v>0.05</v>
       </c>
-      <c r="T22" s="43">
+      <c r="T22" s="34">
         <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="33">
         <v>1E-3</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="32">
         <v>1.61</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="32">
         <v>0.41</v>
       </c>
-      <c r="E23" s="41">
+      <c r="E23" s="32">
         <v>0.1</v>
       </c>
-      <c r="F23" s="41">
+      <c r="F23" s="32">
         <v>0.93</v>
       </c>
-      <c r="G23" s="40"/>
-      <c r="H23" s="41" t="s">
+      <c r="G23" s="31"/>
+      <c r="H23" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="I23" s="42">
+      <c r="I23" s="33">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="J23" s="41">
+      <c r="J23" s="32">
         <v>1.36</v>
       </c>
-      <c r="K23" s="41">
+      <c r="K23" s="32">
         <v>0.47</v>
       </c>
-      <c r="L23" s="41">
+      <c r="L23" s="32">
         <v>0.12</v>
       </c>
-      <c r="M23" s="41">
+      <c r="M23" s="32">
         <v>0.9</v>
       </c>
-      <c r="N23" s="40"/>
-      <c r="O23" s="41" t="s">
+      <c r="N23" s="31"/>
+      <c r="O23" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="P23" s="42">
+      <c r="P23" s="33">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="Q23" s="41">
+      <c r="Q23" s="32">
         <v>1.61</v>
       </c>
-      <c r="R23" s="41">
+      <c r="R23" s="32">
         <v>0.44</v>
       </c>
-      <c r="S23" s="41">
+      <c r="S23" s="32">
         <v>0.12</v>
       </c>
-      <c r="T23" s="41">
+      <c r="T23" s="32">
         <v>0.92</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="42">
+      <c r="B24" s="33">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="32">
         <v>1.7</v>
       </c>
-      <c r="D24" s="41">
+      <c r="D24" s="32">
         <v>0.45</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="32">
         <v>0.18</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="32">
         <v>0.91</v>
       </c>
-      <c r="G24" s="40"/>
-      <c r="H24" s="41" t="s">
+      <c r="G24" s="31"/>
+      <c r="H24" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="42">
+      <c r="I24" s="33">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="J24" s="41">
+      <c r="J24" s="32">
         <v>1.77</v>
       </c>
-      <c r="K24" s="41">
+      <c r="K24" s="32">
         <v>0.46</v>
       </c>
-      <c r="L24" s="41">
+      <c r="L24" s="32">
         <v>0.16</v>
       </c>
-      <c r="M24" s="41">
+      <c r="M24" s="32">
         <v>0.92</v>
       </c>
-      <c r="N24" s="40"/>
-      <c r="O24" s="41" t="s">
+      <c r="N24" s="31"/>
+      <c r="O24" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="P24" s="42">
+      <c r="P24" s="33">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="Q24" s="41">
+      <c r="Q24" s="32">
         <v>2.52</v>
       </c>
-      <c r="R24" s="41">
+      <c r="R24" s="32">
         <v>0.45</v>
       </c>
-      <c r="S24" s="41">
+      <c r="S24" s="32">
         <v>0.18</v>
       </c>
-      <c r="T24" s="41">
+      <c r="T24" s="32">
         <v>0.93</v>
       </c>
     </row>
@@ -10875,7 +11098,7 @@
     </row>
   </sheetData>
   <sortState ref="A1:AI38">
-    <sortCondition sortBy="cellColor" ref="A1:A38" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="A1:A38" dxfId="0"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>